<commit_message>
qr fonctionnel sur 2eme machine (pas encore)
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Liste des Réservations</t>
   </si>
@@ -35,13 +35,16 @@
     <t>Confirmée</t>
   </si>
   <si>
+    <t>monji</t>
+  </si>
+  <si>
+    <t>2025-02-26</t>
+  </si>
+  <si>
+    <t>En attente</t>
+  </si>
+  <si>
     <t>ahmed</t>
-  </si>
-  <si>
-    <t>2025-02-26</t>
-  </si>
-  <si>
-    <t>En attente</t>
   </si>
   <si>
     <t>2025-02-25</t>
@@ -203,10 +206,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>

</xml_diff>

<commit_message>
correction de l'affichage dans backend
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Liste des Réservations</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Confirmée</t>
   </si>
   <si>
-    <t>monji</t>
+    <t>ahmed</t>
   </si>
   <si>
     <t>2025-02-26</t>
@@ -44,10 +44,34 @@
     <t>En attente</t>
   </si>
   <si>
-    <t>ahmed</t>
-  </si>
-  <si>
     <t>2025-02-25</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:34:49.917466400</t>
+  </si>
+  <si>
+    <t>Confirmé</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:40:07.667345</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:44:21.003296400</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:44:34.228014700</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:53:51.661579400</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:58:30.918849200</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:01:30.447345700</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:02:13.757866900</t>
   </si>
 </sst>
 </file>
@@ -155,14 +179,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="19.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="19.58984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="30.8359375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.41796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -206,13 +230,101 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="3">
         <v>10</v>
-      </c>
-      <c r="B5" t="s" s="3">
-        <v>11</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s" s="4">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reservation créée avec création de billet/enlever ajout reservation de backend
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Liste des Réservations</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Confirmée</t>
   </si>
   <si>
-    <t>Utilisateur inconnu</t>
-  </si>
-  <si>
     <t>2025-02-26</t>
   </si>
   <si>
@@ -45,6 +42,12 @@
   </si>
   <si>
     <t>2025-02-25</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:26:34.433205200</t>
+  </si>
+  <si>
+    <t>Confirmé</t>
   </si>
 </sst>
 </file>
@@ -152,14 +155,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="19.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="19.58984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="30.8359375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.41796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -192,24 +195,35 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="C4" t="s" s="0">
         <v>8</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
affichage dans backend corrigé
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Liste des Réservations</t>
   </si>
@@ -35,6 +35,9 @@
     <t>Confirmée</t>
   </si>
   <si>
+    <t>ahmed</t>
+  </si>
+  <si>
     <t>2025-02-26</t>
   </si>
   <si>
@@ -44,10 +47,31 @@
     <t>2025-02-25</t>
   </si>
   <si>
-    <t>2025-03-06T13:26:34.433205200</t>
+    <t>2025-03-06T12:34:49.917466400</t>
   </si>
   <si>
     <t>Confirmé</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:40:07.667345</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:44:21.003296400</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:44:34.228014700</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:53:51.661579400</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:58:30.918849200</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:01:30.447345700</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:02:13.757866900</t>
   </si>
 </sst>
 </file>
@@ -155,7 +179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -195,13 +219,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -209,7 +233,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>
@@ -220,10 +244,87 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s" s="4">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix where remise was applied twice on pdf
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Liste des Réservations</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Confirmée</t>
   </si>
   <si>
-    <t>monji</t>
+    <t>ahmed</t>
   </si>
   <si>
     <t>2025-02-26</t>
@@ -44,10 +44,34 @@
     <t>En attente</t>
   </si>
   <si>
-    <t>ahmed</t>
-  </si>
-  <si>
     <t>2025-02-25</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:34:49.917466400</t>
+  </si>
+  <si>
+    <t>Confirmé</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:40:07.667345</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:44:21.003296400</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:44:34.228014700</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:53:51.661579400</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:58:30.918849200</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:01:30.447345700</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:02:13.757866900</t>
   </si>
 </sst>
 </file>
@@ -155,14 +179,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="19.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="19.58984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="30.8359375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.41796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -206,13 +230,101 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="3">
         <v>10</v>
-      </c>
-      <c r="B5" t="s" s="3">
-        <v>11</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s" s="4">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qrCode now displays ticket owner
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Liste des Réservations</t>
   </si>
@@ -35,43 +35,43 @@
     <t>Confirmée</t>
   </si>
   <si>
+    <t>monji</t>
+  </si>
+  <si>
+    <t>2025-02-26</t>
+  </si>
+  <si>
+    <t>En attente</t>
+  </si>
+  <si>
     <t>ahmed</t>
   </si>
   <si>
-    <t>2025-02-26</t>
-  </si>
-  <si>
-    <t>En attente</t>
-  </si>
-  <si>
     <t>2025-02-25</t>
   </si>
   <si>
-    <t>2025-03-06T12:34:49.917466400</t>
+    <t>2025-03-06T13:56:23.644745200</t>
   </si>
   <si>
     <t>Confirmé</t>
   </si>
   <si>
-    <t>2025-03-06T12:40:07.667345</t>
-  </si>
-  <si>
-    <t>2025-03-06T12:44:21.003296400</t>
-  </si>
-  <si>
-    <t>2025-03-06T12:44:34.228014700</t>
-  </si>
-  <si>
-    <t>2025-03-06T12:53:51.661579400</t>
-  </si>
-  <si>
-    <t>2025-03-06T12:58:30.918849200</t>
-  </si>
-  <si>
-    <t>2025-03-06T13:01:30.447345700</t>
-  </si>
-  <si>
-    <t>2025-03-06T13:02:13.757866900</t>
+    <t>2025-03-06T13:58:54.494560500</t>
+  </si>
+  <si>
+    <t>2025-03-06T14:04:51.406166900</t>
+  </si>
+  <si>
+    <t>2025-03-06T14:07:54.549743800</t>
+  </si>
+  <si>
+    <t>2025-03-06T14:10:38.794597700</t>
+  </si>
+  <si>
+    <t>2025-03-06T14:19:21.469113600</t>
+  </si>
+  <si>
+    <t>2025-03-06T14:24:27.672623800</t>
   </si>
 </sst>
 </file>
@@ -179,7 +179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -230,10 +230,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>
@@ -244,10 +244,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -255,10 +255,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -266,10 +266,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -277,10 +277,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -288,10 +288,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -299,10 +299,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -310,21 +310,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s" s="3">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integration finale avec BD <3
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Liste des Réservations</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Confirmée</t>
   </si>
   <si>
-    <t>monji</t>
+    <t>ahmed</t>
   </si>
   <si>
     <t>2025-02-26</t>
@@ -44,34 +44,49 @@
     <t>En attente</t>
   </si>
   <si>
-    <t>ahmed</t>
-  </si>
-  <si>
     <t>2025-02-25</t>
   </si>
   <si>
-    <t>2025-03-06T13:56:23.644745200</t>
+    <t>2025-03-06T12:34:49.917466400</t>
   </si>
   <si>
     <t>Confirmé</t>
   </si>
   <si>
-    <t>2025-03-06T13:58:54.494560500</t>
-  </si>
-  <si>
-    <t>2025-03-06T14:04:51.406166900</t>
-  </si>
-  <si>
-    <t>2025-03-06T14:07:54.549743800</t>
-  </si>
-  <si>
-    <t>2025-03-06T14:10:38.794597700</t>
-  </si>
-  <si>
-    <t>2025-03-06T14:19:21.469113600</t>
-  </si>
-  <si>
-    <t>2025-03-06T14:24:27.672623800</t>
+    <t>2025-03-06T12:40:07.667345</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:44:21.003296400</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:44:34.228014700</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:53:51.661579400</t>
+  </si>
+  <si>
+    <t>2025-03-06T12:58:30.918849200</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:01:30.447345700</t>
+  </si>
+  <si>
+    <t>2025-03-06T13:02:13.757866900</t>
+  </si>
+  <si>
+    <t>2025-03-06T14:12:36.012794600</t>
+  </si>
+  <si>
+    <t>2025-03-06 14:46:52</t>
+  </si>
+  <si>
+    <t>2025-03-07 08:41:23</t>
+  </si>
+  <si>
+    <t>2025-03-07 09:05:09</t>
+  </si>
+  <si>
+    <t>2025-03-07 09:26:47</t>
   </si>
 </sst>
 </file>
@@ -179,7 +194,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -230,10 +245,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="3">
         <v>10</v>
-      </c>
-      <c r="B5" t="s" s="3">
-        <v>11</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>
@@ -244,10 +259,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -255,10 +270,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -266,10 +281,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -277,10 +292,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -288,10 +303,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -299,10 +314,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -310,10 +325,76 @@
         <v>4</v>
       </c>
       <c r="B12" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="C12" t="s" s="4">
-        <v>13</v>
+      <c r="C13" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s" s="4">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correctionde l'erreur de l'affichage de limage
</commit_message>
<xml_diff>
--- a/reservations.xlsx
+++ b/reservations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>Liste des Réservations</t>
   </si>
@@ -26,24 +26,27 @@
     <t>Statut</t>
   </si>
   <si>
+    <t>raslen</t>
+  </si>
+  <si>
+    <t>2025-04-27 19:04:00</t>
+  </si>
+  <si>
+    <t>Confirmée</t>
+  </si>
+  <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>2025-02-26</t>
+  </si>
+  <si>
+    <t>En attente</t>
+  </si>
+  <si>
     <t>karoui</t>
   </si>
   <si>
-    <t>2025-02-28</t>
-  </si>
-  <si>
-    <t>Confirmée</t>
-  </si>
-  <si>
-    <t>ahmed</t>
-  </si>
-  <si>
-    <t>2025-02-26</t>
-  </si>
-  <si>
-    <t>En attente</t>
-  </si>
-  <si>
     <t>2025-02-25</t>
   </si>
   <si>
@@ -87,6 +90,30 @@
   </si>
   <si>
     <t>2025-03-07 09:26:47</t>
+  </si>
+  <si>
+    <t>2025-03-07 09:52:35</t>
+  </si>
+  <si>
+    <t>2025-04-20 09:31:18</t>
+  </si>
+  <si>
+    <t>confirmée</t>
+  </si>
+  <si>
+    <t>2025-04-20 09:35:25</t>
+  </si>
+  <si>
+    <t>2025-04-20 11:19:35</t>
+  </si>
+  <si>
+    <t>2025-04-20 11:21:09</t>
+  </si>
+  <si>
+    <t>2025-04-22 08:22:58</t>
+  </si>
+  <si>
+    <t>2025-04-22 18:50:50</t>
   </si>
 </sst>
 </file>
@@ -194,7 +221,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -245,10 +272,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>
@@ -256,145 +283,222 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s" s="3">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s" s="3">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s" s="3">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s" s="3">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>